<commit_message>
Mintos: switch to English website
</commit_message>
<xml_diff>
--- a/tests/expected_results/result_test_write_results_mintos_no_cfs.xlsx
+++ b/tests/expected_results/result_test_write_results_mintos_no_cfs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tagesergebnisse" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
   <si>
     <t xml:space="preserve">Plattform</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t xml:space="preserve">Endsaldo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ein-/Auszahlungen</t>
   </si>
   <si>
     <t xml:space="preserve">Investitionen</t>
@@ -211,31 +214,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="34.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -275,13 +279,16 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>42614</v>
@@ -316,10 +323,10 @@
       <c r="M2" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="N2" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -336,30 +343,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="34.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -367,7 +375,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -399,16 +407,19 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -440,12 +451,15 @@
       <c r="M2" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N2" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0</v>
@@ -477,12 +491,15 @@
       <c r="M3" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N3" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0</v>
@@ -514,12 +531,15 @@
       <c r="M4" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N4" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0</v>
@@ -549,6 +569,9 @@
         <v>0</v>
       </c>
       <c r="M5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -572,30 +595,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="34.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -632,13 +656,16 @@
       <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>0</v>
@@ -668,12 +695,15 @@
         <v>0</v>
       </c>
       <c r="L2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="n">
@@ -704,6 +734,9 @@
         <v>0</v>
       </c>
       <c r="L3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>